<commit_message>
added files via commit
</commit_message>
<xml_diff>
--- a/00_documents/visuals/douglas_adjustment/terms_info_aggregated_douglas.xlsx
+++ b/00_documents/visuals/douglas_adjustment/terms_info_aggregated_douglas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65aac5586f718f54/Documents/GitHub/CAN_treaties_NLP/00_documents/visuals/douglas_adjustment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{E0C1DAFE-62E3-410B-AA02-03E94965CE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5F0F77A-C1E0-4BB2-A85C-B553FDCBB920}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{E0C1DAFE-62E3-410B-AA02-03E94965CE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9535CD4A-E0D0-47B0-9C68-6097D5BB2FBF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8E1EB3DC-D270-420F-85B6-D9B25F01A33E}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8E1EB3DC-D270-420F-85B6-D9B25F01A33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="220">
   <si>
     <t>Term</t>
   </si>
@@ -50,9 +50,6 @@
     <t>treati</t>
   </si>
   <si>
-    <t>subject</t>
-  </si>
-  <si>
     <t>becom</t>
   </si>
   <si>
@@ -131,27 +128,12 @@
     <t>acknowledg</t>
   </si>
   <si>
-    <t>abus</t>
-  </si>
-  <si>
     <t>acadi</t>
   </si>
   <si>
-    <t>along</t>
-  </si>
-  <si>
-    <t>wit</t>
-  </si>
-  <si>
-    <t>includ</t>
-  </si>
-  <si>
     <t>confirm</t>
   </si>
   <si>
-    <t>abid</t>
-  </si>
-  <si>
     <t>accru</t>
   </si>
   <si>
@@ -227,9 +209,6 @@
     <t>agre</t>
   </si>
   <si>
-    <t>one</t>
-  </si>
-  <si>
     <t>forev</t>
   </si>
   <si>
@@ -245,24 +224,15 @@
     <t>come</t>
   </si>
   <si>
-    <t>adjut</t>
-  </si>
-  <si>
     <t>affair</t>
   </si>
   <si>
     <t>assist</t>
   </si>
   <si>
-    <t>articl</t>
-  </si>
-  <si>
     <t>five</t>
   </si>
   <si>
-    <t>alexand</t>
-  </si>
-  <si>
     <t>caus</t>
   </si>
   <si>
@@ -281,9 +251,6 @@
     <t>conduct</t>
   </si>
   <si>
-    <t>conclud</t>
-  </si>
-  <si>
     <t>gracious</t>
   </si>
   <si>
@@ -506,9 +473,6 @@
     <t>georg</t>
   </si>
   <si>
-    <t>peac</t>
-  </si>
-  <si>
     <t>control</t>
   </si>
   <si>
@@ -638,72 +602,24 @@
     <t>use</t>
   </si>
   <si>
-    <t>sound</t>
-  </si>
-  <si>
-    <t>return</t>
-  </si>
-  <si>
     <t>affix</t>
   </si>
   <si>
-    <t>acced</t>
-  </si>
-  <si>
     <t>also</t>
   </si>
   <si>
-    <t>britann</t>
-  </si>
-  <si>
-    <t>save</t>
-  </si>
-  <si>
-    <t>aid</t>
-  </si>
-  <si>
-    <t>acr</t>
-  </si>
-  <si>
-    <t>account</t>
-  </si>
-  <si>
     <t>herein</t>
   </si>
   <si>
     <t>district</t>
   </si>
   <si>
-    <t>part</t>
-  </si>
-  <si>
     <t>payment</t>
   </si>
   <si>
-    <t>direct</t>
-  </si>
-  <si>
-    <t>act</t>
-  </si>
-  <si>
-    <t>across</t>
-  </si>
-  <si>
-    <t>citi</t>
-  </si>
-  <si>
     <t>accord</t>
   </si>
   <si>
-    <t>place</t>
-  </si>
-  <si>
-    <t>abl</t>
-  </si>
-  <si>
-    <t>approv</t>
-  </si>
-  <si>
     <t>pay</t>
   </si>
   <si>
@@ -716,34 +632,70 @@
     <t>yield</t>
   </si>
   <si>
-    <t>repres</t>
-  </si>
-  <si>
-    <t>paid</t>
-  </si>
-  <si>
     <t>limit</t>
   </si>
   <si>
-    <t>attach</t>
-  </si>
-  <si>
-    <t>mention</t>
-  </si>
-  <si>
-    <t>twentyf</t>
-  </si>
-  <si>
-    <t>western</t>
-  </si>
-  <si>
-    <t>hereaft</t>
-  </si>
-  <si>
     <t>parti</t>
   </si>
   <si>
     <t>Land vs. Governance/State</t>
+  </si>
+  <si>
+    <t>angl</t>
+  </si>
+  <si>
+    <t>annuiti</t>
+  </si>
+  <si>
+    <t>appoint</t>
+  </si>
+  <si>
+    <t>bay</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>gabriel</t>
+  </si>
+  <si>
+    <t>britain</t>
+  </si>
+  <si>
+    <t>commenc</t>
+  </si>
+  <si>
+    <t>favour</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>aforesaid</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>boundari</t>
+  </si>
+  <si>
+    <t>releas</t>
+  </si>
+  <si>
+    <t>west</t>
+  </si>
+  <si>
+    <t>disturb</t>
+  </si>
+  <si>
+    <t>benefit</t>
+  </si>
+  <si>
+    <t>behalf</t>
+  </si>
+  <si>
+    <t>accur</t>
   </si>
 </sst>
 </file>
@@ -805,6 +757,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1126,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B106625-79B9-4ED7-A7F5-F26762353803}">
   <dimension ref="A1:T107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA71" sqref="AA71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,7 +1105,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1159,64 +1115,64 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C2">
-        <v>16.370591426370702</v>
+        <v>8.8479642616142993</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G2">
-        <v>0.54450239108440901</v>
+        <v>0.53703951150899898</v>
       </c>
       <c r="H2">
-        <v>2.62626262626263E-2</v>
+        <v>7.6187388555681607E-2</v>
       </c>
       <c r="I2">
-        <v>1.3966480446927399E-2</v>
+        <v>4.2826552462526798E-2</v>
       </c>
       <c r="L2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="M2">
         <v>27</v>
@@ -1225,7 +1181,7 @@
         <v>0.78711759748245802</v>
       </c>
       <c r="P2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q2">
         <v>45</v>
@@ -1234,30 +1190,30 @@
         <v>-0.65148517402709405</v>
       </c>
       <c r="T2" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C3">
-        <v>15.6065493383953</v>
+        <v>8.7062409925038704</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="G3">
-        <v>0.166202499102449</v>
+        <v>0.204415995488717</v>
       </c>
       <c r="H3">
-        <v>2.8507295173961798E-2</v>
+        <v>0.11995461176852</v>
       </c>
       <c r="I3">
-        <v>1.67597765363128E-2</v>
+        <v>6.8522483940042803E-2</v>
       </c>
       <c r="L3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="M3">
         <v>34</v>
@@ -1266,7 +1222,7 @@
         <v>0.78447023327508303</v>
       </c>
       <c r="P3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="Q3">
         <v>23</v>
@@ -1277,25 +1233,25 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C4">
-        <v>13.805777429811799</v>
+        <v>6.9084519252212102</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G4">
-        <v>9.7456875107047203E-2</v>
+        <v>7.3680802800183701E-2</v>
       </c>
       <c r="H4">
-        <v>1.2570145903479201E-2</v>
+        <v>9.9935159669314294E-2</v>
       </c>
       <c r="I4">
-        <v>1.3966480446927399E-2</v>
+        <v>6.8522483940042803E-2</v>
       </c>
       <c r="L4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="M4">
         <v>28</v>
@@ -1304,7 +1260,7 @@
         <v>0.776969391203299</v>
       </c>
       <c r="P4" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="Q4">
         <v>27</v>
@@ -1318,22 +1274,22 @@
         <v>44</v>
       </c>
       <c r="C5">
-        <v>13.5089567754963</v>
+        <v>6.8381236333486903</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G5">
-        <v>3.2007544872290898E-2</v>
+        <v>4.5183252135359397E-2</v>
       </c>
       <c r="H5">
-        <v>4.6127946127946101E-2</v>
+        <v>1.84794942454207E-2</v>
       </c>
       <c r="I5">
-        <v>3.0726256983240201E-2</v>
+        <v>1.7130620985010701E-2</v>
       </c>
       <c r="L5" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="M5">
         <v>30</v>
@@ -1342,7 +1298,7 @@
         <v>0.71906548266008996</v>
       </c>
       <c r="P5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="Q5">
         <v>30</v>
@@ -1353,25 +1309,25 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C6">
-        <v>12.984159215746301</v>
+        <v>6.6966475431446399</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="G6">
-        <v>2.6537038692544299E-2</v>
+        <v>3.4464922687839003E-2</v>
       </c>
       <c r="H6">
-        <v>1.9079685746352399E-3</v>
+        <v>7.2945372021397297E-3</v>
       </c>
       <c r="I6">
-        <v>2.7932960893854702E-3</v>
+        <v>6.4239828693790097E-3</v>
       </c>
       <c r="L6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M6">
         <v>43</v>
@@ -1380,7 +1336,7 @@
         <v>0.71138783892356605</v>
       </c>
       <c r="P6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="Q6">
         <v>12</v>
@@ -1391,25 +1347,25 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="C7">
-        <v>12.938852441459501</v>
+        <v>6.4838447971972002</v>
       </c>
       <c r="F7" t="s">
-        <v>129</v>
+        <v>39</v>
       </c>
       <c r="G7">
-        <v>1.7876090677578501E-2</v>
+        <v>2.86185453566183E-2</v>
       </c>
       <c r="H7">
-        <v>6.17283950617284E-3</v>
+        <v>1.5399578537850501E-2</v>
       </c>
       <c r="I7">
-        <v>5.5865921787709499E-3</v>
+        <v>1.2847965738758E-2</v>
       </c>
       <c r="L7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M7">
         <v>24</v>
@@ -1418,7 +1374,7 @@
         <v>0.70584575933892402</v>
       </c>
       <c r="P7" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="Q7">
         <v>15</v>
@@ -1429,25 +1385,25 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8">
-        <v>12.2669544505865</v>
+        <v>6.1317015271724102</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="G8">
-        <v>1.6593404125933301E-2</v>
+        <v>2.8017836106353899E-2</v>
       </c>
       <c r="H8">
-        <v>6.6217732884399604E-3</v>
+        <v>1.21575620035662E-2</v>
       </c>
       <c r="I8">
-        <v>8.3798882681564192E-3</v>
+        <v>1.9271948608137E-2</v>
       </c>
       <c r="L8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="M8">
         <v>42</v>
@@ -1456,7 +1412,7 @@
         <v>0.69582848050837898</v>
       </c>
       <c r="P8" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="Q8">
         <v>20</v>
@@ -1467,25 +1423,25 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="C9">
-        <v>10.2607588203477</v>
+        <v>5.33801702531151</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="G9">
-        <v>1.6012444426657502E-2</v>
+        <v>1.5842534487400101E-2</v>
       </c>
       <c r="H9">
-        <v>1.9079685746352399E-3</v>
+        <v>5.8356297617117798E-3</v>
       </c>
       <c r="I9">
-        <v>2.7932960893854702E-3</v>
+        <v>8.5653104925053503E-3</v>
       </c>
       <c r="L9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M9">
         <v>26</v>
@@ -1494,7 +1450,7 @@
         <v>0.694066861382443</v>
       </c>
       <c r="P9" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="Q9">
         <v>11</v>
@@ -1505,25 +1461,25 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C10">
-        <v>8.2766585497525806</v>
+        <v>5.1144026670613103</v>
       </c>
       <c r="F10" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="G10">
-        <v>1.1801752796088701E-2</v>
+        <v>4.77698426320725E-3</v>
       </c>
       <c r="H10">
-        <v>2.2446689113355799E-3</v>
+        <v>6.9703355487112997E-3</v>
       </c>
       <c r="I10">
-        <v>2.7932960893854702E-3</v>
+        <v>8.5653104925053503E-3</v>
       </c>
       <c r="L10" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="M10">
         <v>26</v>
@@ -1532,7 +1488,7 @@
         <v>0.66728095522668196</v>
       </c>
       <c r="P10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="Q10">
         <v>30</v>
@@ -1543,25 +1499,25 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C11">
-        <v>7.9597244397937503</v>
+        <v>4.4355996210265198</v>
       </c>
       <c r="F11" t="s">
-        <v>7</v>
+        <v>187</v>
       </c>
       <c r="G11">
-        <v>7.9364270482036193E-3</v>
+        <v>4.2598452517093504E-3</v>
       </c>
       <c r="H11">
-        <v>6.7340067340067302E-3</v>
+        <v>1.1266007456638E-2</v>
       </c>
       <c r="I11">
-        <v>1.11731843575419E-2</v>
+        <v>1.2847965738758E-2</v>
       </c>
       <c r="L11" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="M11">
         <v>14</v>
@@ -1570,7 +1526,7 @@
         <v>0.66575614048396703</v>
       </c>
       <c r="P11" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="Q11">
         <v>16</v>
@@ -1581,25 +1537,25 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C12">
-        <v>7.7969516136305197</v>
+        <v>3.9480640521043</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>201</v>
       </c>
       <c r="G12">
-        <v>7.8603981279493293E-3</v>
+        <v>3.1640821676331599E-3</v>
       </c>
       <c r="H12">
-        <v>4.4893378226711599E-3</v>
+        <v>3.40411736099854E-3</v>
       </c>
       <c r="I12">
-        <v>1.11731843575419E-2</v>
+        <v>4.2826552462526804E-3</v>
       </c>
       <c r="L12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M12">
         <v>27</v>
@@ -1608,7 +1564,7 @@
         <v>0.66169947769130499</v>
       </c>
       <c r="P12" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="Q12">
         <v>10</v>
@@ -1619,25 +1575,25 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13">
+        <v>3.6879639418446901</v>
+      </c>
+      <c r="F13" t="s">
+        <v>202</v>
+      </c>
+      <c r="G13">
+        <v>2.9765347640098101E-3</v>
+      </c>
+      <c r="H13">
+        <v>2.7557140541416801E-3</v>
+      </c>
+      <c r="I13">
+        <v>4.2826552462526804E-3</v>
+      </c>
+      <c r="L13" t="s">
         <v>48</v>
-      </c>
-      <c r="C13">
-        <v>7.7720452728153404</v>
-      </c>
-      <c r="F13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G13">
-        <v>7.46313372785144E-3</v>
-      </c>
-      <c r="H13">
-        <v>3.9281705948372601E-3</v>
-      </c>
-      <c r="I13">
-        <v>1.3966480446927399E-2</v>
-      </c>
-      <c r="L13" t="s">
-        <v>54</v>
       </c>
       <c r="M13">
         <v>29</v>
@@ -1646,7 +1602,7 @@
         <v>0.65551485982660795</v>
       </c>
       <c r="P13" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="Q13">
         <v>15</v>
@@ -1657,25 +1613,25 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>129</v>
+        <v>49</v>
       </c>
       <c r="C14">
-        <v>7.3742665477287899</v>
+        <v>3.6693033697559199</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="G14">
-        <v>7.3847837429700898E-3</v>
+        <v>2.7814533488621498E-3</v>
       </c>
       <c r="H14">
-        <v>3.4792368125701502E-3</v>
+        <v>8.5102934024963509E-3</v>
       </c>
       <c r="I14">
-        <v>5.5865921787709499E-3</v>
+        <v>1.49892933618844E-2</v>
       </c>
       <c r="L14" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M14">
         <v>31</v>
@@ -1684,7 +1640,7 @@
         <v>0.64878701252768001</v>
       </c>
       <c r="P14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="Q14">
         <v>13</v>
@@ -1695,25 +1651,25 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>7.2461864302191499</v>
+        <v>3.5758275478904702</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G15">
-        <v>6.7208075472050604E-3</v>
+        <v>1.69138767805228E-3</v>
       </c>
       <c r="H15">
-        <v>1.1896745230078601E-2</v>
+        <v>5.9409952990760302E-2</v>
       </c>
       <c r="I15">
-        <v>8.3798882681564192E-3</v>
+        <v>4.92505353319058E-2</v>
       </c>
       <c r="L15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="M15">
         <v>41</v>
@@ -1722,7 +1678,7 @@
         <v>0.64602260189101801</v>
       </c>
       <c r="P15" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="Q15">
         <v>34</v>
@@ -1733,25 +1689,25 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C16">
-        <v>7.1261773057451698</v>
+        <v>3.3248015222885501</v>
       </c>
       <c r="F16" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G16">
-        <v>5.3388147162056702E-3</v>
+        <v>1.31977050361817E-3</v>
       </c>
       <c r="H16">
-        <v>1.4141414141414101E-2</v>
+        <v>4.1335710812125098E-3</v>
       </c>
       <c r="I16">
-        <v>1.11731843575419E-2</v>
+        <v>6.4239828693790097E-3</v>
       </c>
       <c r="L16" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="M16">
         <v>30</v>
@@ -1760,7 +1716,7 @@
         <v>0.63679297227920495</v>
       </c>
       <c r="P16" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="Q16">
         <v>14</v>
@@ -1771,25 +1727,25 @@
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="C17">
-        <v>6.4876552966554497</v>
+        <v>3.20862479897368</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="G17">
-        <v>3.7815364662368901E-3</v>
+        <v>9.3339377546944801E-4</v>
       </c>
       <c r="H17">
-        <v>1.35802469135802E-2</v>
+        <v>4.9440752147835998E-3</v>
       </c>
       <c r="I17">
-        <v>1.3966480446927399E-2</v>
+        <v>1.07066381156317E-2</v>
       </c>
       <c r="L17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="M17">
         <v>10</v>
@@ -1798,7 +1754,7 @@
         <v>0.63410941085223504</v>
       </c>
       <c r="P17" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="Q17">
         <v>15</v>
@@ -1809,25 +1765,25 @@
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>55</v>
+        <v>187</v>
       </c>
       <c r="C18">
-        <v>6.2558207546226798</v>
+        <v>3.0112665170478099</v>
       </c>
       <c r="F18" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G18">
-        <v>3.6352450524090598E-3</v>
+        <v>8.5263209911187602E-4</v>
       </c>
       <c r="H18">
-        <v>4.71380471380471E-3</v>
+        <v>1.7831090938563801E-3</v>
       </c>
       <c r="I18">
-        <v>5.5865921787709499E-3</v>
+        <v>2.1413276231263402E-3</v>
       </c>
       <c r="L18" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="M18">
         <v>20</v>
@@ -1836,7 +1792,7 @@
         <v>0.62990124185977403</v>
       </c>
       <c r="P18" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="Q18">
         <v>19</v>
@@ -1847,25 +1803,25 @@
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>199</v>
+        <v>94</v>
       </c>
       <c r="C19">
-        <v>5.88347378178059</v>
+        <v>2.7941543062073602</v>
       </c>
       <c r="F19" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="G19">
-        <v>3.2747384052846601E-3</v>
+        <v>8.2037119692441804E-4</v>
       </c>
       <c r="H19">
-        <v>1.08866442199776E-2</v>
+        <v>6.9703355487112997E-3</v>
       </c>
       <c r="I19">
-        <v>1.11731843575419E-2</v>
+        <v>6.4239828693790097E-3</v>
       </c>
       <c r="L19" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="M19">
         <v>19</v>
@@ -1874,7 +1830,7 @@
         <v>0.61845268315865298</v>
       </c>
       <c r="P19" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="Q19">
         <v>12</v>
@@ -1885,25 +1841,25 @@
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C20">
-        <v>5.8388208589418698</v>
+        <v>2.7938263157102199</v>
       </c>
       <c r="F20" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="G20">
-        <v>3.0760296717361902E-3</v>
+        <v>7.8504504625545699E-4</v>
       </c>
       <c r="H20">
-        <v>3.3670033670033699E-3</v>
+        <v>6.9703355487112997E-3</v>
       </c>
       <c r="I20">
-        <v>2.7932960893854702E-3</v>
+        <v>6.4239828693790097E-3</v>
       </c>
       <c r="L20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="M20">
         <v>39</v>
@@ -1912,7 +1868,7 @@
         <v>0.61151725599209905</v>
       </c>
       <c r="P20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q20">
         <v>13</v>
@@ -1923,25 +1879,25 @@
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="C21">
-        <v>5.3798897722769201</v>
+        <v>2.6395217033678202</v>
       </c>
       <c r="F21" t="s">
-        <v>203</v>
+        <v>81</v>
       </c>
       <c r="G21">
-        <v>2.4536062558759399E-3</v>
+        <v>7.12530498960739E-4</v>
       </c>
       <c r="H21">
-        <v>0.179349046015713</v>
+        <v>6.24088182849733E-3</v>
       </c>
       <c r="I21">
-        <v>9.4972067039106101E-2</v>
+        <v>1.07066381156317E-2</v>
       </c>
       <c r="L21" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="M21">
         <v>36</v>
@@ -1950,7 +1906,7 @@
         <v>0.60664102436353495</v>
       </c>
       <c r="P21" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="Q21">
         <v>14</v>
@@ -1961,25 +1917,25 @@
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C22">
-        <v>5.3741758931342796</v>
+        <v>2.5042432869543201</v>
       </c>
       <c r="F22" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="G22">
-        <v>2.41981095889275E-3</v>
+        <v>6.2457415522420396E-4</v>
       </c>
       <c r="H22">
-        <v>1.9079685746352399E-3</v>
+        <v>1.6210082671421599E-3</v>
       </c>
       <c r="I22">
-        <v>5.5865921787709499E-3</v>
+        <v>4.2826552462526804E-3</v>
       </c>
       <c r="L22" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="M22">
         <v>13</v>
@@ -1988,7 +1944,7 @@
         <v>0.60635092171348903</v>
       </c>
       <c r="P22" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="Q22">
         <v>11</v>
@@ -1999,25 +1955,25 @@
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>200</v>
+        <v>45</v>
       </c>
       <c r="C23">
-        <v>5.3457448757983803</v>
+        <v>2.4809232645178501</v>
       </c>
       <c r="F23" t="s">
-        <v>114</v>
+        <v>188</v>
       </c>
       <c r="G23">
-        <v>2.13468862354326E-3</v>
+        <v>4.7045033785172102E-4</v>
       </c>
       <c r="H23">
-        <v>2.3569023569023598E-3</v>
+        <v>9.0857513373318197E-2</v>
       </c>
       <c r="I23">
-        <v>2.7932960893854702E-3</v>
+        <v>5.5674518201284801E-2</v>
       </c>
       <c r="L23" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="M23">
         <v>24</v>
@@ -2026,7 +1982,7 @@
         <v>0.59928244513240803</v>
       </c>
       <c r="P23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q23">
         <v>18</v>
@@ -2037,25 +1993,25 @@
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="C24">
-        <v>5.1987422129158798</v>
+        <v>2.4547978170058999</v>
       </c>
       <c r="F24" t="s">
-        <v>204</v>
+        <v>14</v>
       </c>
       <c r="G24">
-        <v>1.07073354361491E-3</v>
+        <v>4.33955230584318E-4</v>
       </c>
       <c r="H24">
-        <v>4.3771043771043804E-3</v>
+        <v>4.0525206678554103E-3</v>
       </c>
       <c r="I24">
-        <v>1.11731843575419E-2</v>
+        <v>6.4239828693790097E-3</v>
       </c>
       <c r="L24" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="M24">
         <v>35</v>
@@ -2064,7 +2020,7 @@
         <v>0.59312363423900405</v>
       </c>
       <c r="P24" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="Q24">
         <v>12</v>
@@ -2075,25 +2031,25 @@
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C25">
-        <v>5.0190218966378799</v>
+        <v>2.4314331818094499</v>
       </c>
       <c r="F25" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="G25">
-        <v>7.1733545322423802E-4</v>
+        <v>4.2378107421673402E-4</v>
       </c>
       <c r="H25">
-        <v>6.0606060606060597E-3</v>
+        <v>2.6665585994488601E-2</v>
       </c>
       <c r="I25">
-        <v>1.95530726256983E-2</v>
+        <v>1.49892933618844E-2</v>
       </c>
       <c r="L25" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M25">
         <v>32</v>
@@ -2113,25 +2069,25 @@
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="C26">
-        <v>5.0164120947037496</v>
+        <v>2.42626919842672</v>
       </c>
       <c r="F26" t="s">
-        <v>34</v>
+        <v>193</v>
       </c>
       <c r="G26">
-        <v>5.8441526297395004E-4</v>
+        <v>3.8716407068516899E-4</v>
       </c>
       <c r="H26">
-        <v>5.1627384960718304E-3</v>
+        <v>4.5388231479980496E-3</v>
       </c>
       <c r="I26">
-        <v>5.5865921787709499E-3</v>
+        <v>6.4239828693790097E-3</v>
       </c>
       <c r="L26" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M26">
         <v>21</v>
@@ -2140,7 +2096,7 @@
         <v>0.55535594350966799</v>
       </c>
       <c r="P26" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="Q26">
         <v>13</v>
@@ -2151,25 +2107,25 @@
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>156</v>
+        <v>61</v>
       </c>
       <c r="C27">
-        <v>4.9919443471465099</v>
+        <v>2.3560816133284801</v>
       </c>
       <c r="F27" t="s">
+        <v>111</v>
+      </c>
+      <c r="G27">
+        <v>3.4867405334500001E-4</v>
+      </c>
+      <c r="H27">
+        <v>4.8630248014264899E-3</v>
+      </c>
+      <c r="I27">
+        <v>4.2826552462526804E-3</v>
+      </c>
+      <c r="L27" t="s">
         <v>174</v>
-      </c>
-      <c r="G27">
-        <v>5.7760306189849598E-4</v>
-      </c>
-      <c r="H27">
-        <v>2.1324354657688001E-3</v>
-      </c>
-      <c r="I27">
-        <v>2.7932960893854702E-3</v>
-      </c>
-      <c r="L27" t="s">
-        <v>186</v>
       </c>
       <c r="M27">
         <v>21</v>
@@ -2178,7 +2134,7 @@
         <v>0.55393435341238595</v>
       </c>
       <c r="P27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q27">
         <v>20</v>
@@ -2189,25 +2145,25 @@
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>157</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>4.9048033910207502</v>
+        <v>2.34820025248847</v>
       </c>
       <c r="F28" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="G28">
-        <v>5.1859531046302395E-4</v>
+        <v>3.0789361983712401E-4</v>
       </c>
       <c r="H28">
-        <v>7.8563411896745202E-3</v>
+        <v>1.7020586804992702E-2</v>
       </c>
       <c r="I28">
-        <v>4.18994413407821E-2</v>
+        <v>1.7130620985010701E-2</v>
       </c>
       <c r="L28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M28">
         <v>25</v>
@@ -2216,7 +2172,7 @@
         <v>0.54218506687944401</v>
       </c>
       <c r="P28" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="Q28">
         <v>21</v>
@@ -2227,25 +2183,25 @@
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C29">
-        <v>4.7554050007064896</v>
+        <v>2.2679364870290701</v>
       </c>
       <c r="F29" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="G29">
-        <v>3.9337939372674399E-4</v>
+        <v>2.8630052252443601E-4</v>
       </c>
       <c r="H29">
-        <v>1.3468013468013499E-3</v>
+        <v>2.9988652942130002E-3</v>
       </c>
       <c r="I29">
-        <v>5.5865921787709499E-3</v>
+        <v>4.2826552462526804E-3</v>
       </c>
       <c r="L29" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="M29">
         <v>21</v>
@@ -2254,7 +2210,7 @@
         <v>0.54132779589320701</v>
       </c>
       <c r="P29" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="Q29">
         <v>13</v>
@@ -2265,25 +2221,25 @@
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
       <c r="C30">
-        <v>4.7419927223077902</v>
+        <v>2.2667746124774899</v>
       </c>
       <c r="F30" t="s">
-        <v>158</v>
+        <v>30</v>
       </c>
       <c r="G30">
-        <v>3.50438766855543E-4</v>
+        <v>2.6692340729704903E-4</v>
       </c>
       <c r="H30">
-        <v>1.79573512906846E-3</v>
+        <v>8.9155454692818896E-4</v>
       </c>
       <c r="I30">
-        <v>5.5865921787709499E-3</v>
+        <v>2.1413276231263402E-3</v>
       </c>
       <c r="L30" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="M30">
         <v>12</v>
@@ -2292,7 +2248,7 @@
         <v>0.53543112634413803</v>
       </c>
       <c r="P30" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="Q30">
         <v>12</v>
@@ -2303,25 +2259,25 @@
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>123</v>
+        <v>4</v>
       </c>
       <c r="C31">
-        <v>4.7234815544837101</v>
+        <v>2.2188446664287498</v>
       </c>
       <c r="F31" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="G31">
-        <v>2.97136676703362E-4</v>
+        <v>2.3214998893055199E-4</v>
       </c>
       <c r="H31">
-        <v>1.7059483726150401E-2</v>
+        <v>3.3230669476414301E-3</v>
       </c>
       <c r="I31">
-        <v>1.3966480446927399E-2</v>
+        <v>1.07066381156317E-2</v>
       </c>
       <c r="L31" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="M31">
         <v>31</v>
@@ -2330,7 +2286,7 @@
         <v>0.52992377812684399</v>
       </c>
       <c r="P31" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="Q31">
         <v>21</v>
@@ -2341,25 +2297,25 @@
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="C32">
-        <v>4.56823716732411</v>
+        <v>2.1351368124299199</v>
       </c>
       <c r="F32" t="s">
         <v>205</v>
       </c>
       <c r="G32">
-        <v>2.8695568940424499E-4</v>
+        <v>2.2998427424406501E-4</v>
       </c>
       <c r="H32">
-        <v>2.2446689113355799E-3</v>
+        <v>5.5114281082833498E-3</v>
       </c>
       <c r="I32">
-        <v>2.7932960893854702E-3</v>
+        <v>8.5653104925053503E-3</v>
       </c>
       <c r="L32" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="M32">
         <v>36</v>
@@ -2368,7 +2324,7 @@
         <v>0.52731255336481897</v>
       </c>
       <c r="P32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q32">
         <v>20</v>
@@ -2379,25 +2335,25 @@
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="C33">
-        <v>4.48492829850598</v>
+        <v>2.1109523645555299</v>
       </c>
       <c r="F33" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="G33">
-        <v>2.78687595123163E-4</v>
+        <v>2.2723261766684999E-4</v>
       </c>
       <c r="H33">
-        <v>1.9079685746352399E-3</v>
+        <v>1.53185281244934E-2</v>
       </c>
       <c r="I33">
-        <v>2.7932960893854702E-3</v>
+        <v>3.2119914346895102E-2</v>
       </c>
       <c r="L33" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="M33">
         <v>19</v>
@@ -2406,7 +2362,7 @@
         <v>0.52659201656849297</v>
       </c>
       <c r="P33" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="Q33">
         <v>13</v>
@@ -2417,25 +2373,25 @@
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="C34">
-        <v>4.4554393143290003</v>
+        <v>2.0263137028726899</v>
       </c>
       <c r="F34" t="s">
-        <v>74</v>
+        <v>206</v>
       </c>
       <c r="G34">
-        <v>2.7197199219256902E-4</v>
+        <v>2.24767511398443E-4</v>
       </c>
       <c r="H34">
-        <v>3.1537598204264897E-2</v>
+        <v>1.70205868049927E-3</v>
       </c>
       <c r="I34">
-        <v>2.5139664804469299E-2</v>
+        <v>2.1413276231263402E-3</v>
       </c>
       <c r="L34" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="M34">
         <v>21</v>
@@ -2444,7 +2400,7 @@
         <v>0.52309721978971102</v>
       </c>
       <c r="P34" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="Q34">
         <v>12</v>
@@ -2455,25 +2411,25 @@
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
       <c r="C35">
-        <v>4.4355436434868096</v>
+        <v>1.9894635716315101</v>
       </c>
       <c r="F35" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G35">
-        <v>2.4216452230527299E-4</v>
+        <v>2.19033020480588E-4</v>
       </c>
       <c r="H35">
-        <v>2.1324354657688001E-3</v>
+        <v>5.8356297617117798E-3</v>
       </c>
       <c r="I35">
-        <v>2.7932960893854702E-3</v>
+        <v>6.4239828693790097E-3</v>
       </c>
       <c r="L35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M35">
         <v>26</v>
@@ -2482,7 +2438,7 @@
         <v>0.49697145595354197</v>
       </c>
       <c r="P35" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="Q35">
         <v>12</v>
@@ -2493,25 +2449,25 @@
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>170</v>
+        <v>58</v>
       </c>
       <c r="C36">
-        <v>4.4104920514544199</v>
+        <v>1.9798217533439799</v>
       </c>
       <c r="F36" t="s">
-        <v>207</v>
+        <v>158</v>
       </c>
       <c r="G36">
-        <v>2.12503050227627E-4</v>
+        <v>2.1643291531928E-4</v>
       </c>
       <c r="H36">
-        <v>1.5712682379349001E-3</v>
+        <v>1.0536553736424099E-2</v>
       </c>
       <c r="I36">
-        <v>2.7932960893854702E-3</v>
+        <v>1.49892933618844E-2</v>
       </c>
       <c r="L36" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="M36">
         <v>26</v>
@@ -2520,7 +2476,7 @@
         <v>0.49389813666357602</v>
       </c>
       <c r="P36" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="Q36">
         <v>13</v>
@@ -2530,26 +2486,8 @@
       </c>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>120</v>
-      </c>
-      <c r="C37">
-        <v>4.2555585588208</v>
-      </c>
-      <c r="F37" t="s">
-        <v>208</v>
-      </c>
-      <c r="G37">
-        <v>1.95173673217439E-4</v>
-      </c>
-      <c r="H37">
-        <v>2.2446689113355799E-3</v>
-      </c>
-      <c r="I37">
-        <v>1.11731843575419E-2</v>
-      </c>
       <c r="L37" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="M37">
         <v>34</v>
@@ -2558,7 +2496,7 @@
         <v>0.484056745960251</v>
       </c>
       <c r="P37" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="Q37">
         <v>25</v>
@@ -2568,26 +2506,8 @@
       </c>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38">
-        <v>4.1670783907136704</v>
-      </c>
-      <c r="F38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G38">
-        <v>1.5702193535858E-4</v>
-      </c>
-      <c r="H38">
-        <v>2.58136924803591E-3</v>
-      </c>
-      <c r="I38">
-        <v>2.7932960893854702E-3</v>
-      </c>
       <c r="L38" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="M38">
         <v>10</v>
@@ -2596,7 +2516,7 @@
         <v>0.47819363278725302</v>
       </c>
       <c r="P38" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="Q38">
         <v>15</v>
@@ -2606,26 +2526,8 @@
       </c>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>118</v>
-      </c>
-      <c r="C39">
-        <v>3.9665767739031201</v>
-      </c>
-      <c r="F39" t="s">
-        <v>37</v>
-      </c>
-      <c r="G39">
-        <v>1.48586572203959E-4</v>
-      </c>
-      <c r="H39">
-        <v>2.1324354657688001E-3</v>
-      </c>
-      <c r="I39">
-        <v>2.7932960893854702E-3</v>
-      </c>
       <c r="L39" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="M39">
         <v>26</v>
@@ -2634,7 +2536,7 @@
         <v>0.47313224358092199</v>
       </c>
       <c r="P39" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="Q39">
         <v>12</v>
@@ -2644,26 +2546,8 @@
       </c>
     </row>
     <row r="40" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40">
-        <v>3.9339576536819001</v>
-      </c>
-      <c r="F40" t="s">
-        <v>69</v>
-      </c>
-      <c r="G40">
-        <v>1.4292119895062801E-4</v>
-      </c>
-      <c r="H40">
-        <v>2.0202020202020202E-3</v>
-      </c>
-      <c r="I40">
-        <v>8.3798882681564192E-3</v>
-      </c>
       <c r="L40" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="M40">
         <v>14</v>
@@ -2682,26 +2566,8 @@
       </c>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41">
-        <v>3.6842508477145302</v>
-      </c>
-      <c r="F41" t="s">
-        <v>209</v>
-      </c>
-      <c r="G41">
-        <v>1.0414786980839501E-4</v>
-      </c>
-      <c r="H41">
-        <v>8.97867564534231E-4</v>
-      </c>
-      <c r="I41">
-        <v>2.7932960893854702E-3</v>
-      </c>
       <c r="P41" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="Q41">
         <v>12</v>
@@ -2711,14 +2577,8 @@
       </c>
     </row>
     <row r="42" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>154</v>
-      </c>
-      <c r="C42">
-        <v>3.6755654574794998</v>
-      </c>
       <c r="P42" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="Q42">
         <v>13</v>
@@ -2728,14 +2588,8 @@
       </c>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43">
-        <v>3.6705039911524899</v>
-      </c>
       <c r="P43" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="Q43">
         <v>13</v>
@@ -2745,14 +2599,8 @@
       </c>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44">
-        <v>3.5395533844340101</v>
-      </c>
       <c r="P44" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="Q44">
         <v>15</v>
@@ -2762,14 +2610,8 @@
       </c>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>201</v>
-      </c>
-      <c r="C45">
-        <v>3.5359316877869902</v>
-      </c>
       <c r="P45" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="Q45">
         <v>11</v>
@@ -2779,14 +2621,8 @@
       </c>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>2</v>
-      </c>
-      <c r="C46">
-        <v>3.4862221178477699</v>
-      </c>
       <c r="P46" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="Q46">
         <v>14</v>
@@ -2797,7 +2633,7 @@
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P47" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="Q47">
         <v>13</v>
@@ -2808,7 +2644,7 @@
     </row>
     <row r="48" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P48" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="Q48">
         <v>14</v>
@@ -2819,7 +2655,7 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B49" t="s">
         <v>0</v>
@@ -2829,22 +2665,22 @@
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G49" t="s">
+        <v>24</v>
+      </c>
+      <c r="H49" t="s">
         <v>25</v>
       </c>
-      <c r="H49" t="s">
+      <c r="I49" t="s">
         <v>26</v>
       </c>
-      <c r="I49" t="s">
-        <v>27</v>
-      </c>
       <c r="P49" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="Q49">
         <v>13</v>
@@ -2855,25 +2691,25 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C50">
-        <v>11.485180312829099</v>
+        <v>6.5026639208104404</v>
       </c>
       <c r="F50" t="s">
-        <v>8</v>
+        <v>166</v>
       </c>
       <c r="G50">
-        <v>0.27910862878660497</v>
+        <v>0.40596290149298803</v>
       </c>
       <c r="H50">
-        <v>2.1937445699391801E-2</v>
+        <v>0.113090800656031</v>
       </c>
       <c r="I50">
-        <v>1.3698630136986301E-2</v>
+        <v>6.8041237113402098E-2</v>
       </c>
       <c r="P50" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="Q50">
         <v>14</v>
@@ -2884,25 +2720,25 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C51">
-        <v>11.2334289272415</v>
+        <v>5.7182658385033802</v>
       </c>
       <c r="F51" t="s">
-        <v>178</v>
+        <v>18</v>
       </c>
       <c r="G51">
-        <v>0.25549937593271899</v>
+        <v>0.10786152476868099</v>
       </c>
       <c r="H51">
-        <v>7.4934839270199803E-3</v>
+        <v>1.9159087520501002E-2</v>
       </c>
       <c r="I51">
-        <v>5.4794520547945197E-3</v>
+        <v>1.4432989690721701E-2</v>
       </c>
       <c r="P51" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="Q51">
         <v>12</v>
@@ -2913,86 +2749,86 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C52">
-        <v>10.862621627088799</v>
+        <v>5.6068154913662802</v>
       </c>
       <c r="F52" t="s">
-        <v>160</v>
+        <v>16</v>
       </c>
       <c r="G52">
-        <v>9.8943211206592496E-2</v>
+        <v>9.5357495353631999E-2</v>
       </c>
       <c r="H52">
-        <v>3.1602953953084302E-2</v>
+        <v>4.2045623974951499E-2</v>
       </c>
       <c r="I52">
-        <v>1.9178082191780799E-2</v>
+        <v>2.4742268041237098E-2</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C53">
-        <v>10.718272001066101</v>
+        <v>5.5211771622349204</v>
       </c>
       <c r="F53" t="s">
-        <v>202</v>
+        <v>52</v>
       </c>
       <c r="G53">
-        <v>8.7409269005588999E-2</v>
+        <v>9.4617407065120201E-2</v>
       </c>
       <c r="H53">
-        <v>8.3297132927888803E-2</v>
+        <v>1.75190099895631E-2</v>
       </c>
       <c r="I53">
-        <v>7.1232876712328794E-2</v>
+        <v>3.09278350515464E-2</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R53" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
       <c r="C54">
-        <v>9.8713808004396899</v>
+        <v>5.13891919014692</v>
       </c>
       <c r="F54" t="s">
-        <v>19</v>
+        <v>176</v>
       </c>
       <c r="G54">
-        <v>7.1899655772830598E-2</v>
+        <v>8.0814716118373806E-2</v>
       </c>
       <c r="H54">
-        <v>1.78105994787142E-2</v>
+        <v>4.6816758610407003E-2</v>
       </c>
       <c r="I54">
-        <v>1.3698630136986301E-2</v>
+        <v>2.88659793814433E-2</v>
       </c>
       <c r="L54" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="M54">
         <v>37</v>
@@ -3001,7 +2837,7 @@
         <v>0.69680749928363295</v>
       </c>
       <c r="P54" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="Q54">
         <v>27</v>
@@ -3012,25 +2848,25 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C55">
-        <v>8.1352841923653898</v>
+        <v>4.66054001665771</v>
       </c>
       <c r="F55" t="s">
-        <v>58</v>
+        <v>148</v>
       </c>
       <c r="G55">
-        <v>6.8824056477195694E-2</v>
+        <v>5.0228113205029901E-2</v>
       </c>
       <c r="H55">
-        <v>1.0860121633362301E-3</v>
+        <v>4.79349932905919E-2</v>
       </c>
       <c r="I55">
-        <v>2.7397260273972599E-3</v>
+        <v>3.09278350515464E-2</v>
       </c>
       <c r="L55" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="M55">
         <v>14</v>
@@ -3039,7 +2875,7 @@
         <v>0.69124763543134404</v>
       </c>
       <c r="P55" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="Q55">
         <v>21</v>
@@ -3050,25 +2886,25 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="C56">
-        <v>7.5745277603269896</v>
+        <v>4.1176638343406697</v>
       </c>
       <c r="F56" t="s">
-        <v>62</v>
+        <v>195</v>
       </c>
       <c r="G56">
-        <v>2.02096542666023E-2</v>
+        <v>3.5432975926716299E-2</v>
       </c>
       <c r="H56">
-        <v>1.11859252823632E-2</v>
+        <v>3.5038019979126301E-3</v>
       </c>
       <c r="I56">
-        <v>8.21917808219178E-3</v>
+        <v>2.0618556701030898E-3</v>
       </c>
       <c r="L56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M56">
         <v>18</v>
@@ -3077,7 +2913,7 @@
         <v>0.68186505637523198</v>
       </c>
       <c r="P56" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="Q56">
         <v>13</v>
@@ -3088,25 +2924,25 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="C57">
-        <v>7.3140966544908697</v>
+        <v>4.0223465234567</v>
       </c>
       <c r="F57" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="G57">
-        <v>1.40721090352226E-2</v>
+        <v>2.64460877054979E-2</v>
       </c>
       <c r="H57">
-        <v>5.3540399652476103E-2</v>
+        <v>0.101610257939466</v>
       </c>
       <c r="I57">
-        <v>3.5616438356164397E-2</v>
+        <v>5.97938144329897E-2</v>
       </c>
       <c r="L57" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="M57">
         <v>11</v>
@@ -3115,7 +2951,7 @@
         <v>0.64933882879619798</v>
       </c>
       <c r="P57" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="Q57">
         <v>13</v>
@@ -3126,25 +2962,25 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>158</v>
+        <v>16</v>
       </c>
       <c r="C58">
-        <v>7.1012512254819899</v>
+        <v>3.9737285176578099</v>
       </c>
       <c r="F58" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="G58">
-        <v>1.32110796837387E-2</v>
+        <v>2.1372933120888799E-2</v>
       </c>
       <c r="H58">
-        <v>6.1902693310165102E-3</v>
+        <v>2.1619203816907701E-2</v>
       </c>
       <c r="I58">
-        <v>1.0958904109589E-2</v>
+        <v>4.3298969072164899E-2</v>
       </c>
       <c r="L58" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="M58">
         <v>12</v>
@@ -3153,7 +2989,7 @@
         <v>0.64474667941994701</v>
       </c>
       <c r="P58" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="Q58">
         <v>27</v>
@@ -3164,25 +3000,25 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>188</v>
+        <v>31</v>
       </c>
       <c r="C59">
-        <v>7.0435887801596904</v>
+        <v>3.6499837895410501</v>
       </c>
       <c r="F59" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G59">
-        <v>1.22198545582536E-2</v>
+        <v>1.28182436996541E-2</v>
       </c>
       <c r="H59">
-        <v>2.9322328410078201E-3</v>
+        <v>1.3791561055613501E-2</v>
       </c>
       <c r="I59">
-        <v>2.7397260273972599E-3</v>
+        <v>1.03092783505155E-2</v>
       </c>
       <c r="L59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M59">
         <v>27</v>
@@ -3191,7 +3027,7 @@
         <v>0.63794994751205203</v>
       </c>
       <c r="P59" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="Q59">
         <v>15</v>
@@ -3202,25 +3038,25 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="C60">
-        <v>6.8974478702312503</v>
+        <v>3.6076566993655299</v>
       </c>
       <c r="F60" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G60">
-        <v>1.0469936619272599E-2</v>
+        <v>1.24370697628861E-2</v>
       </c>
       <c r="H60">
-        <v>4.7784535186794104E-3</v>
+        <v>8.2003876546891301E-4</v>
       </c>
       <c r="I60">
-        <v>5.4794520547945197E-3</v>
+        <v>2.0618556701030898E-3</v>
       </c>
       <c r="L60" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="M60">
         <v>36</v>
@@ -3229,7 +3065,7 @@
         <v>0.60879203663923598</v>
       </c>
       <c r="P60" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="Q60">
         <v>13</v>
@@ -3240,25 +3076,25 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>223</v>
+        <v>119</v>
       </c>
       <c r="C61">
-        <v>6.8241960868770404</v>
+        <v>3.5444002470995</v>
       </c>
       <c r="F61" t="s">
-        <v>95</v>
+        <v>211</v>
       </c>
       <c r="G61">
-        <v>1.01216839870268E-2</v>
+        <v>1.2042370797680399E-2</v>
       </c>
       <c r="H61">
-        <v>5.8644656820156403E-3</v>
+        <v>7.9021917399731603E-3</v>
       </c>
       <c r="I61">
-        <v>5.4794520547945197E-3</v>
+        <v>1.85567010309278E-2</v>
       </c>
       <c r="L61" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M61">
         <v>20</v>
@@ -3267,7 +3103,7 @@
         <v>0.60485657906885004</v>
       </c>
       <c r="P61" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="Q61">
         <v>15</v>
@@ -3278,25 +3114,25 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
+        <v>188</v>
+      </c>
+      <c r="C62">
+        <v>3.4764458387711001</v>
+      </c>
+      <c r="F62" t="s">
         <v>212</v>
       </c>
-      <c r="C62">
-        <v>6.4027007624782399</v>
-      </c>
-      <c r="F62" t="s">
-        <v>30</v>
-      </c>
       <c r="G62">
-        <v>9.4799092672431303E-3</v>
+        <v>6.7293215834126801E-3</v>
       </c>
       <c r="H62">
-        <v>6.4074717636837496E-3</v>
+        <v>2.3855673177277498E-3</v>
       </c>
       <c r="I62">
-        <v>1.9178082191780799E-2</v>
+        <v>4.12371134020619E-3</v>
       </c>
       <c r="L62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M62">
         <v>20</v>
@@ -3305,7 +3141,7 @@
         <v>0.59857579977929698</v>
       </c>
       <c r="P62" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="Q62">
         <v>16</v>
@@ -3316,25 +3152,25 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C63">
-        <v>6.33683381038077</v>
+        <v>3.38956949063921</v>
       </c>
       <c r="F63" t="s">
-        <v>212</v>
+        <v>119</v>
       </c>
       <c r="G63">
-        <v>5.7077320076123301E-3</v>
+        <v>5.8105280963496502E-3</v>
       </c>
       <c r="H63">
-        <v>1.00999131190269E-2</v>
+        <v>1.64007753093783E-2</v>
       </c>
       <c r="I63">
-        <v>1.6438356164383602E-2</v>
+        <v>1.85567010309278E-2</v>
       </c>
       <c r="L63" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="M63">
         <v>15</v>
@@ -3343,7 +3179,7 @@
         <v>0.57866060513085704</v>
       </c>
       <c r="P63" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="Q63">
         <v>14</v>
@@ -3354,25 +3190,25 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
       <c r="C64">
-        <v>6.1456382281713697</v>
+        <v>3.1528239136137102</v>
       </c>
       <c r="F64" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="G64">
-        <v>4.8491874072966101E-3</v>
+        <v>5.55514035713588E-3</v>
       </c>
       <c r="H64">
-        <v>4.6698523023457903E-3</v>
+        <v>1.1331444759206799E-2</v>
       </c>
       <c r="I64">
-        <v>2.7397260273972599E-3</v>
+        <v>2.6804123711340201E-2</v>
       </c>
       <c r="L64" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="M64">
         <v>14</v>
@@ -3392,25 +3228,25 @@
     </row>
     <row r="65" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C65">
-        <v>6.1186200565017801</v>
+        <v>3.1457118762699898</v>
       </c>
       <c r="F65" t="s">
-        <v>36</v>
+        <v>138</v>
       </c>
       <c r="G65">
-        <v>4.6706448910112499E-3</v>
+        <v>4.5844148805721701E-3</v>
       </c>
       <c r="H65">
-        <v>4.1268462206776697E-3</v>
+        <v>5.3675264648874298E-3</v>
       </c>
       <c r="I65">
-        <v>5.4794520547945197E-3</v>
+        <v>6.1855670103092798E-3</v>
       </c>
       <c r="L65" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="M65">
         <v>16</v>
@@ -3419,7 +3255,7 @@
         <v>0.56903129667750596</v>
       </c>
       <c r="P65" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="Q65">
         <v>12</v>
@@ -3430,25 +3266,25 @@
     </row>
     <row r="66" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C66">
-        <v>6.0032879000539001</v>
+        <v>3.08726657951091</v>
       </c>
       <c r="F66" t="s">
-        <v>130</v>
+        <v>213</v>
       </c>
       <c r="G66">
-        <v>4.0201643073372803E-3</v>
+        <v>3.31011437710495E-3</v>
       </c>
       <c r="H66">
-        <v>1.00999131190269E-2</v>
+        <v>7.0821529745042503E-3</v>
       </c>
       <c r="I66">
-        <v>1.3698630136986301E-2</v>
+        <v>6.1855670103092798E-3</v>
       </c>
       <c r="L66" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="M66">
         <v>21</v>
@@ -3457,7 +3293,7 @@
         <v>0.56669694021607897</v>
       </c>
       <c r="P66" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="Q66">
         <v>37</v>
@@ -3468,25 +3304,25 @@
     </row>
     <row r="67" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>224</v>
+        <v>166</v>
       </c>
       <c r="C67">
-        <v>5.69827252213015</v>
+        <v>3.0530194498021399</v>
       </c>
       <c r="F67" t="s">
-        <v>68</v>
+        <v>214</v>
       </c>
       <c r="G67">
-        <v>3.6164230906867399E-3</v>
+        <v>2.8199697496805402E-3</v>
       </c>
       <c r="H67">
-        <v>3.4752389226759299E-3</v>
+        <v>7.7530937826151801E-3</v>
       </c>
       <c r="I67">
-        <v>5.4794520547945197E-3</v>
+        <v>6.1855670103092798E-3</v>
       </c>
       <c r="L67" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M67">
         <v>21</v>
@@ -3495,7 +3331,7 @@
         <v>0.52019519175389095</v>
       </c>
       <c r="P67" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="Q67">
         <v>13</v>
@@ -3506,25 +3342,25 @@
     </row>
     <row r="68" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>170</v>
+        <v>18</v>
       </c>
       <c r="C68">
-        <v>5.60322531576531</v>
+        <v>2.7729873451728202</v>
       </c>
       <c r="F68" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="G68">
-        <v>3.3070336486231301E-3</v>
+        <v>2.5146309761465801E-3</v>
       </c>
       <c r="H68">
-        <v>2.7150304083405699E-3</v>
+        <v>1.8786342627106E-2</v>
       </c>
       <c r="I68">
-        <v>2.7397260273972599E-3</v>
+        <v>1.2371134020618599E-2</v>
       </c>
       <c r="L68" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="M68">
         <v>16</v>
@@ -3533,7 +3369,7 @@
         <v>0.51484937355247895</v>
       </c>
       <c r="P68" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="Q68">
         <v>16</v>
@@ -3544,25 +3380,25 @@
     </row>
     <row r="69" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>225</v>
+        <v>154</v>
       </c>
       <c r="C69">
-        <v>5.4986726947438598</v>
+        <v>2.7611205345924299</v>
       </c>
       <c r="F69" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="G69">
-        <v>2.9553095168013402E-3</v>
+        <v>1.50483139797338E-3</v>
       </c>
       <c r="H69">
-        <v>0.16072980017376201</v>
+        <v>4.0256448486655702E-3</v>
       </c>
       <c r="I69">
-        <v>0.106849315068493</v>
+        <v>4.12371134020619E-3</v>
       </c>
       <c r="L69" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="M69">
         <v>25</v>
@@ -3571,7 +3407,7 @@
         <v>0.49250644842997099</v>
       </c>
       <c r="P69" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="Q69">
         <v>13</v>
@@ -3582,25 +3418,25 @@
     </row>
     <row r="70" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>213</v>
+        <v>158</v>
       </c>
       <c r="C70">
-        <v>5.3558002991611904</v>
+        <v>2.7438587468030802</v>
       </c>
       <c r="F70" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="G70">
-        <v>2.1682935658602501E-3</v>
+        <v>1.30190290716081E-3</v>
       </c>
       <c r="H70">
-        <v>6.5160729800173801E-3</v>
+        <v>4.9202325928134798E-3</v>
       </c>
       <c r="I70">
-        <v>1.0958904109589E-2</v>
+        <v>1.2371134020618599E-2</v>
       </c>
       <c r="L70" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="M70">
         <v>11</v>
@@ -3609,7 +3445,7 @@
         <v>0.48161912095055798</v>
       </c>
       <c r="P70" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="Q70">
         <v>12</v>
@@ -3620,25 +3456,25 @@
     </row>
     <row r="71" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C71">
-        <v>5.3133163424410697</v>
+        <v>2.7024201554422298</v>
       </c>
       <c r="F71" t="s">
-        <v>6</v>
+        <v>130</v>
       </c>
       <c r="G71">
-        <v>2.11898483229683E-3</v>
+        <v>1.1860496268902899E-3</v>
       </c>
       <c r="H71">
-        <v>4.8870547350130297E-3</v>
+        <v>7.0076039958252602E-3</v>
       </c>
       <c r="I71">
-        <v>5.4794520547945197E-3</v>
+        <v>1.2371134020618599E-2</v>
       </c>
       <c r="L71" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="M71">
         <v>21</v>
@@ -3647,7 +3483,7 @@
         <v>0.46592588588432898</v>
       </c>
       <c r="P71" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="Q71">
         <v>12</v>
@@ -3658,25 +3494,25 @@
     </row>
     <row r="72" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>226</v>
+        <v>91</v>
       </c>
       <c r="C72">
-        <v>5.2564838565492797</v>
+        <v>2.7016343406125598</v>
       </c>
       <c r="F72" t="s">
-        <v>33</v>
+        <v>190</v>
       </c>
       <c r="G72">
-        <v>1.73390557841684E-3</v>
+        <v>9.7890413771212193E-4</v>
       </c>
       <c r="H72">
-        <v>1.2380538662033E-2</v>
+        <v>2.2364693603697601E-3</v>
       </c>
       <c r="I72">
-        <v>8.21917808219178E-3</v>
+        <v>2.0618556701030898E-3</v>
       </c>
       <c r="L72" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="M72">
         <v>15</v>
@@ -3685,7 +3521,7 @@
         <v>0.463645186800069</v>
       </c>
       <c r="P72" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="Q72">
         <v>12</v>
@@ -3696,25 +3532,25 @@
     </row>
     <row r="73" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="C73">
-        <v>5.1740586900698498</v>
+        <v>2.6293808030946502</v>
       </c>
       <c r="F73" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="G73">
-        <v>1.2801268647929099E-3</v>
+        <v>5.4075120738183101E-4</v>
       </c>
       <c r="H73">
-        <v>1.62901824500434E-3</v>
+        <v>5.7999105412255801E-2</v>
       </c>
       <c r="I73">
-        <v>2.7397260273972599E-3</v>
+        <v>4.9484536082474197E-2</v>
       </c>
       <c r="L73" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="M73">
         <v>13</v>
@@ -3723,7 +3559,7 @@
         <v>0.45264093425841601</v>
       </c>
       <c r="P73" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="Q73">
         <v>23</v>
@@ -3734,25 +3570,25 @@
     </row>
     <row r="74" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C74">
-        <v>5.1678298880475504</v>
+        <v>2.49639574899328</v>
       </c>
       <c r="F74" t="s">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="G74">
-        <v>1.24758479827273E-3</v>
+        <v>5.1447140734596898E-4</v>
       </c>
       <c r="H74">
-        <v>8.0364900086880992E-3</v>
+        <v>5.5166244222454204E-3</v>
       </c>
       <c r="I74">
-        <v>8.21917808219178E-3</v>
+        <v>1.2371134020618599E-2</v>
       </c>
       <c r="L74" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M74">
         <v>32</v>
@@ -3761,7 +3597,7 @@
         <v>0.45069816968251297</v>
       </c>
       <c r="P74" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="Q74">
         <v>33</v>
@@ -3772,25 +3608,25 @@
     </row>
     <row r="75" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>227</v>
+        <v>58</v>
       </c>
       <c r="C75">
-        <v>4.95769959631349</v>
+        <v>2.3816004667828299</v>
       </c>
       <c r="F75" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="G75">
-        <v>1.1772070606462599E-3</v>
+        <v>5.0116680597403604E-4</v>
       </c>
       <c r="H75">
-        <v>3.58384013900956E-3</v>
+        <v>2.08737140301178E-3</v>
       </c>
       <c r="I75">
-        <v>1.3698630136986301E-2</v>
+        <v>2.0618556701030898E-3</v>
       </c>
       <c r="L75" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="M75">
         <v>12</v>
@@ -3799,7 +3635,7 @@
         <v>0.41595601449998498</v>
       </c>
       <c r="P75" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="Q75">
         <v>12</v>
@@ -3810,25 +3646,25 @@
     </row>
     <row r="76" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>102</v>
+        <v>199</v>
       </c>
       <c r="C76">
-        <v>4.7613500353590599</v>
+        <v>2.3725802560869602</v>
       </c>
       <c r="F76" t="s">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="G76">
-        <v>9.9212384854722394E-4</v>
+        <v>4.2913592835530802E-4</v>
       </c>
       <c r="H76">
-        <v>2.9322328410078201E-3</v>
+        <v>8.7222305054420798E-3</v>
       </c>
       <c r="I76">
-        <v>2.7397260273972599E-3</v>
+        <v>6.1855670103092798E-3</v>
       </c>
       <c r="L76" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M76">
         <v>23</v>
@@ -3837,7 +3673,7 @@
         <v>0.41222413583325301</v>
       </c>
       <c r="P76" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="Q76">
         <v>10</v>
@@ -3848,25 +3684,25 @@
     </row>
     <row r="77" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="C77">
-        <v>4.7319570726802498</v>
+        <v>2.3154516634621101</v>
       </c>
       <c r="F77" t="s">
-        <v>207</v>
+        <v>136</v>
       </c>
       <c r="G77">
-        <v>7.9642189140991795E-4</v>
+        <v>3.9994300019940602E-4</v>
       </c>
       <c r="H77">
-        <v>6.5160729800173799E-4</v>
+        <v>3.5783509765916202E-3</v>
       </c>
       <c r="I77">
-        <v>2.7397260273972599E-3</v>
+        <v>4.12371134020619E-3</v>
       </c>
       <c r="L77" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="M77">
         <v>21</v>
@@ -3875,7 +3711,7 @@
         <v>0.40848192255157201</v>
       </c>
       <c r="P77" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="Q77">
         <v>26</v>
@@ -3886,25 +3722,25 @@
     </row>
     <row r="78" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>128</v>
+        <v>192</v>
       </c>
       <c r="C78">
-        <v>4.6424267185926498</v>
+        <v>2.2949425056169499</v>
       </c>
       <c r="F78" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="G78">
-        <v>7.6598963327621002E-4</v>
+        <v>3.8280102026817998E-4</v>
       </c>
       <c r="H78">
-        <v>4.4417897480451801E-2</v>
+        <v>6.1130162516773497E-3</v>
       </c>
       <c r="I78">
-        <v>4.65753424657534E-2</v>
+        <v>8.2474226804123696E-3</v>
       </c>
       <c r="L78" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="M78">
         <v>14</v>
@@ -3913,7 +3749,7 @@
         <v>0.40329211515767199</v>
       </c>
       <c r="P78" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="Q78">
         <v>12</v>
@@ -3924,25 +3760,25 @@
     </row>
     <row r="79" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>116</v>
+        <v>2</v>
       </c>
       <c r="C79">
-        <v>4.5951912886333099</v>
+        <v>2.2774576246115901</v>
       </c>
       <c r="F79" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="G79">
-        <v>7.3008988120137203E-4</v>
+        <v>3.6052559024335598E-4</v>
       </c>
       <c r="H79">
-        <v>1.4118158123371E-3</v>
+        <v>3.7274489339495999E-3</v>
       </c>
       <c r="I79">
-        <v>5.4794520547945197E-3</v>
+        <v>1.03092783505155E-2</v>
       </c>
       <c r="L79" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="M79">
         <v>12</v>
@@ -3951,7 +3787,7 @@
         <v>0.39269750217425597</v>
       </c>
       <c r="P79" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="Q79">
         <v>22</v>
@@ -3962,25 +3798,25 @@
     </row>
     <row r="80" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>73</v>
+        <v>208</v>
       </c>
       <c r="C80">
-        <v>4.4777785991109997</v>
+        <v>2.25517252260323</v>
       </c>
       <c r="F80" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G80">
-        <v>7.1322177870103605E-4</v>
+        <v>3.5990177587036598E-4</v>
       </c>
       <c r="H80">
-        <v>3.2580364900086899E-4</v>
+        <v>4.3238407633815401E-3</v>
       </c>
       <c r="I80">
-        <v>2.7397260273972599E-3</v>
+        <v>6.1855670103092798E-3</v>
       </c>
       <c r="L80" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="M80">
         <v>15</v>
@@ -3989,7 +3825,7 @@
         <v>0.37658383143993102</v>
       </c>
       <c r="P80" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="Q80">
         <v>12</v>
@@ -4000,25 +3836,25 @@
     </row>
     <row r="81" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>165</v>
+        <v>8</v>
       </c>
       <c r="C81">
-        <v>4.4388367914979998</v>
+        <v>2.2476977406251</v>
       </c>
       <c r="F81" t="s">
-        <v>217</v>
+        <v>22</v>
       </c>
       <c r="G81">
-        <v>6.6815550330890695E-4</v>
+        <v>3.4435675743295499E-4</v>
       </c>
       <c r="H81">
-        <v>4.7784535186794104E-3</v>
+        <v>2.0128224243327899E-3</v>
       </c>
       <c r="I81">
-        <v>2.7397260273972599E-3</v>
+        <v>2.0618556701030898E-3</v>
       </c>
       <c r="L81" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M81">
         <v>18</v>
@@ -4027,7 +3863,7 @@
         <v>0.37219284286339899</v>
       </c>
       <c r="P81" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="Q81">
         <v>13</v>
@@ -4038,25 +3874,25 @@
     </row>
     <row r="82" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>228</v>
+        <v>84</v>
       </c>
       <c r="C82">
-        <v>4.4296487961301603</v>
+        <v>2.1787196380739999</v>
       </c>
       <c r="F82" t="s">
-        <v>218</v>
+        <v>180</v>
       </c>
       <c r="G82">
-        <v>6.1838871374669997E-4</v>
+        <v>3.3045763843395201E-4</v>
       </c>
       <c r="H82">
-        <v>5.1042571676802803E-3</v>
+        <v>4.4580289250037299E-2</v>
       </c>
       <c r="I82">
-        <v>2.46575342465753E-2</v>
+        <v>2.88659793814433E-2</v>
       </c>
       <c r="L82" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="M82">
         <v>16</v>
@@ -4065,7 +3901,7 @@
         <v>0.37084308471065203</v>
       </c>
       <c r="P82" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q82">
         <v>16</v>
@@ -4076,25 +3912,25 @@
     </row>
     <row r="83" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>229</v>
+        <v>151</v>
       </c>
       <c r="C83">
-        <v>4.2008127225472602</v>
+        <v>2.1658271039527799</v>
       </c>
       <c r="F83" t="s">
-        <v>219</v>
+        <v>114</v>
       </c>
       <c r="G83">
-        <v>4.8857839448237595E-4</v>
+        <v>3.2411410894477699E-4</v>
       </c>
       <c r="H83">
-        <v>1.62901824500434E-3</v>
+        <v>1.71462650961682E-3</v>
       </c>
       <c r="I83">
-        <v>2.7397260273972599E-3</v>
+        <v>2.0618556701030898E-3</v>
       </c>
       <c r="L83" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="M83">
         <v>10</v>
@@ -4103,7 +3939,7 @@
         <v>0.36396274172030901</v>
       </c>
       <c r="P83" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="Q83">
         <v>25</v>
@@ -4114,25 +3950,25 @@
     </row>
     <row r="84" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="C84">
-        <v>4.0220866093254601</v>
+        <v>2.1623413623018899</v>
       </c>
       <c r="F84" t="s">
-        <v>194</v>
+        <v>105</v>
       </c>
       <c r="G84">
-        <v>4.6735225142306599E-4</v>
+        <v>3.08078885800981E-4</v>
       </c>
       <c r="H84">
-        <v>9.7741094700260593E-3</v>
+        <v>1.70717161174892E-2</v>
       </c>
       <c r="I84">
-        <v>5.4794520547945197E-3</v>
+        <v>1.6494845360824701E-2</v>
       </c>
       <c r="L84" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="M84">
         <v>13</v>
@@ -4141,7 +3977,7 @@
         <v>0.35415421985732798</v>
       </c>
       <c r="P84" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="Q84">
         <v>14</v>
@@ -4151,26 +3987,8 @@
       </c>
     </row>
     <row r="85" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>36</v>
-      </c>
-      <c r="C85">
-        <v>3.9867952209491202</v>
-      </c>
-      <c r="F85" t="s">
-        <v>220</v>
-      </c>
-      <c r="G85">
-        <v>4.4808359164007601E-4</v>
-      </c>
-      <c r="H85">
-        <v>1.19461337966985E-3</v>
-      </c>
-      <c r="I85">
-        <v>2.7397260273972599E-3</v>
-      </c>
       <c r="L85" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="M85">
         <v>23</v>
@@ -4179,7 +3997,7 @@
         <v>0.35185754205771003</v>
       </c>
       <c r="P85" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="Q85">
         <v>13</v>
@@ -4189,26 +4007,8 @@
       </c>
     </row>
     <row r="86" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>123</v>
-      </c>
-      <c r="C86">
-        <v>3.9645093064716601</v>
-      </c>
-      <c r="F86" t="s">
-        <v>31</v>
-      </c>
-      <c r="G86">
-        <v>3.72605173281156E-4</v>
-      </c>
-      <c r="H86">
-        <v>1.19461337966985E-3</v>
-      </c>
-      <c r="I86">
-        <v>5.4794520547945197E-3</v>
-      </c>
       <c r="L86" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="M86">
         <v>11</v>
@@ -4217,7 +4017,7 @@
         <v>0.35034196488115299</v>
       </c>
       <c r="P86" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="Q86">
         <v>12</v>
@@ -4227,26 +4027,8 @@
       </c>
     </row>
     <row r="87" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>72</v>
-      </c>
-      <c r="C87">
-        <v>3.8120848135536498</v>
-      </c>
-      <c r="F87" t="s">
-        <v>221</v>
-      </c>
-      <c r="G87">
-        <v>3.1068683348880902E-4</v>
-      </c>
-      <c r="H87">
-        <v>9.7741094700260606E-4</v>
-      </c>
-      <c r="I87">
-        <v>2.7397260273972599E-3</v>
-      </c>
       <c r="L87" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="M87">
         <v>35</v>
@@ -4255,7 +4037,7 @@
         <v>0.337717733437921</v>
       </c>
       <c r="P87" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="Q87">
         <v>12</v>
@@ -4265,26 +4047,8 @@
       </c>
     </row>
     <row r="88" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>11</v>
-      </c>
-      <c r="C88">
-        <v>3.7708174584640699</v>
-      </c>
-      <c r="F88" t="s">
-        <v>138</v>
-      </c>
-      <c r="G88">
-        <v>2.2637235526909701E-4</v>
-      </c>
-      <c r="H88">
-        <v>4.28974804517811E-2</v>
-      </c>
-      <c r="I88">
-        <v>2.46575342465753E-2</v>
-      </c>
       <c r="L88" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="M88">
         <v>15</v>
@@ -4293,7 +4057,7 @@
         <v>0.33263253578549401</v>
       </c>
       <c r="P88" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="Q88">
         <v>16</v>
@@ -4303,14 +4067,8 @@
       </c>
     </row>
     <row r="89" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>35</v>
-      </c>
-      <c r="C89">
-        <v>3.7316588869507799</v>
-      </c>
       <c r="L89" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="M89">
         <v>34</v>
@@ -4319,7 +4077,7 @@
         <v>0.33166649276540699</v>
       </c>
       <c r="P89" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="Q89">
         <v>26</v>
@@ -4329,14 +4087,8 @@
       </c>
     </row>
     <row r="90" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>9</v>
-      </c>
-      <c r="C90">
-        <v>3.6868135362455101</v>
-      </c>
       <c r="L90" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="M90">
         <v>10</v>
@@ -4345,7 +4097,7 @@
         <v>0.32603682630314201</v>
       </c>
       <c r="P90" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="Q90">
         <v>37</v>
@@ -4355,14 +4107,8 @@
       </c>
     </row>
     <row r="91" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>162</v>
-      </c>
-      <c r="C91">
-        <v>3.6818109818087699</v>
-      </c>
       <c r="L91" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="M91">
         <v>15</v>
@@ -4371,7 +4117,7 @@
         <v>0.31706721264993498</v>
       </c>
       <c r="P91" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="Q91">
         <v>13</v>
@@ -4381,14 +4127,8 @@
       </c>
     </row>
     <row r="92" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>230</v>
-      </c>
-      <c r="C92">
-        <v>3.6122450665638399</v>
-      </c>
       <c r="L92" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="M92">
         <v>15</v>
@@ -4397,7 +4137,7 @@
         <v>0.31123101564227301</v>
       </c>
       <c r="P92" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="Q92">
         <v>10</v>
@@ -4407,14 +4147,8 @@
       </c>
     </row>
     <row r="93" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>231</v>
-      </c>
-      <c r="C93">
-        <v>3.5249129881712902</v>
-      </c>
       <c r="L93" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="M93">
         <v>30</v>
@@ -4423,7 +4157,7 @@
         <v>0.30755693950789198</v>
       </c>
       <c r="P93" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="Q93">
         <v>15</v>
@@ -4433,14 +4167,8 @@
       </c>
     </row>
     <row r="94" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>175</v>
-      </c>
-      <c r="C94">
-        <v>3.5219143012071399</v>
-      </c>
       <c r="L94" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="M94">
         <v>10</v>
@@ -4449,7 +4177,7 @@
         <v>0.30596824237589099</v>
       </c>
       <c r="P94" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Q94">
         <v>28</v>
@@ -4459,14 +4187,8 @@
       </c>
     </row>
     <row r="95" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>232</v>
-      </c>
-      <c r="C95">
-        <v>3.50625113395918</v>
-      </c>
       <c r="L95" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="M95">
         <v>15</v>
@@ -4475,7 +4197,7 @@
         <v>0.30409564178769999</v>
       </c>
       <c r="P95" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="Q95">
         <v>41</v>
@@ -4485,14 +4207,8 @@
       </c>
     </row>
     <row r="96" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>233</v>
-      </c>
-      <c r="C96">
-        <v>3.4936543450427799</v>
-      </c>
       <c r="L96" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="M96">
         <v>17</v>
@@ -4501,7 +4217,7 @@
         <v>0.30190136104985699</v>
       </c>
       <c r="P96" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="Q96">
         <v>13</v>
@@ -4510,15 +4226,9 @@
         <v>-0.40323121335479201</v>
       </c>
     </row>
-    <row r="97" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>95</v>
-      </c>
-      <c r="C97">
-        <v>3.4327840060615999</v>
-      </c>
+    <row r="97" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L97" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="M97">
         <v>20</v>
@@ -4527,7 +4237,7 @@
         <v>0.30108577004791898</v>
       </c>
       <c r="P97" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="Q97">
         <v>13</v>
@@ -4536,15 +4246,9 @@
         <v>-0.40077600343540398</v>
       </c>
     </row>
-    <row r="98" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
-        <v>234</v>
-      </c>
-      <c r="C98">
-        <v>3.4126962572465702</v>
-      </c>
+    <row r="98" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L98" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="M98">
         <v>15</v>
@@ -4553,7 +4257,7 @@
         <v>0.28918734300356302</v>
       </c>
       <c r="P98" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="Q98">
         <v>12</v>
@@ -4562,15 +4266,9 @@
         <v>-0.40073079324932198</v>
       </c>
     </row>
-    <row r="99" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>53</v>
-      </c>
-      <c r="C99">
-        <v>3.3470375360576701</v>
-      </c>
+    <row r="99" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L99" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="M99">
         <v>18</v>
@@ -4579,7 +4277,7 @@
         <v>0.27957606794742801</v>
       </c>
       <c r="P99" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="Q99">
         <v>11</v>
@@ -4588,15 +4286,9 @@
         <v>-0.39951484501187101</v>
       </c>
     </row>
-    <row r="100" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100">
-        <v>3.3442727148937101</v>
-      </c>
+    <row r="100" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L100" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="M100">
         <v>10</v>
@@ -4605,7 +4297,7 @@
         <v>0.27814071002799201</v>
       </c>
       <c r="P100" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="Q100">
         <v>11</v>
@@ -4614,15 +4306,9 @@
         <v>-0.39723698278057801</v>
       </c>
     </row>
-    <row r="101" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>6</v>
-      </c>
-      <c r="C101">
-        <v>3.2837960426431501</v>
-      </c>
+    <row r="101" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L101" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="M101">
         <v>10</v>
@@ -4631,7 +4317,7 @@
         <v>0.27717398495657503</v>
       </c>
       <c r="P101" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="Q101">
         <v>12</v>
@@ -4640,15 +4326,9 @@
         <v>-0.39522038961212602</v>
       </c>
     </row>
-    <row r="102" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>10</v>
-      </c>
-      <c r="C102">
-        <v>3.2775049343915201</v>
-      </c>
+    <row r="102" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L102" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="M102">
         <v>15</v>
@@ -4657,7 +4337,7 @@
         <v>0.268001678102809</v>
       </c>
       <c r="P102" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="Q102">
         <v>29</v>
@@ -4666,9 +4346,9 @@
         <v>-0.394817083384152</v>
       </c>
     </row>
-    <row r="103" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L103" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="M103">
         <v>27</v>
@@ -4677,9 +4357,9 @@
         <v>0.26564427051098299</v>
       </c>
     </row>
-    <row r="104" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L104" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="M104">
         <v>35</v>
@@ -4688,9 +4368,9 @@
         <v>0.26373610091218203</v>
       </c>
     </row>
-    <row r="105" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L105" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M105">
         <v>25</v>
@@ -4699,9 +4379,9 @@
         <v>0.25835850486227502</v>
       </c>
     </row>
-    <row r="106" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="106" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L106" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="M106">
         <v>18</v>
@@ -4710,9 +4390,9 @@
         <v>0.24772292054235501</v>
       </c>
     </row>
-    <row r="107" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L107" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="M107">
         <v>23</v>

</xml_diff>